<commit_message>
add save as dialog to export feature
</commit_message>
<xml_diff>
--- a/SIMS_TEMPLATE.xlsx
+++ b/SIMS_TEMPLATE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="7665"/>
+    <workbookView windowWidth="19800" windowHeight="7665" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Cresdel Pharmacy Latest Inventory</t>
   </si>
@@ -105,19 +105,13 @@
     <t>no_reply@example.com</t>
   </si>
   <si>
+    <t>Batch #</t>
+  </si>
+  <si>
     <t>Item Name</t>
   </si>
   <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
-    <t>Shipping &amp; handling</t>
-  </si>
-  <si>
-    <t>Tax rate</t>
-  </si>
-  <si>
-    <t>Sales tax</t>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -126,12 +120,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -219,13 +213,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color rgb="FF666666"/>
       <name val="Roboto"/>
@@ -270,36 +257,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -320,10 +287,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -335,86 +340,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -427,6 +357,50 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -434,7 +408,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,14 +441,182 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCEDDE1"/>
-        <bgColor rgb="FFCEDDE1"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -483,188 +625,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -679,15 +641,6 @@
       <bottom style="thin">
         <color rgb="FFB7B7B7"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFB7B7B7"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -706,13 +659,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -728,6 +685,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -750,8 +727,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -760,31 +737,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,152 +759,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="34" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="34" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1019,10 +972,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1030,56 +980,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1134,91 +1077,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-        <charset val="134"/>
-        <family val="0"/>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-        <charset val="134"/>
-        <family val="0"/>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-        <charset val="134"/>
-        <family val="0"/>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-        <charset val="134"/>
-        <family val="0"/>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-        <charset val="134"/>
-        <family val="0"/>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-        <charset val="134"/>
-        <family val="0"/>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -1324,12 +1183,12 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="Sales Report-style" pivot="0" count="2">
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="secondRowStripe" dxfId="5"/>
     </tableStyle>
     <tableStyle name="Purchase order Report-style" pivot="0" count="2">
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="secondRowStripe" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="secondRowStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1350,20 +1209,6 @@
     <tableColumn id="5" name="Column5" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Sales Report-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" displayName="Table_2" ref="B28:G33" headerRowCount="0">
-  <tableColumns count="6">
-    <tableColumn id="1" name="Column1" dataDxfId="5"/>
-    <tableColumn id="2" name="Column2" dataDxfId="6"/>
-    <tableColumn id="3" name="Column3" dataDxfId="7"/>
-    <tableColumn id="4" name="Column4" dataDxfId="8"/>
-    <tableColumn id="5" name="Column5" dataDxfId="9"/>
-    <tableColumn id="6" name="Column6" dataDxfId="10"/>
-  </tableColumns>
-  <tableStyleInfo name="Purchase order Report-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1628,13 +1473,13 @@
     <tabColor rgb="FF76A5AF"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="2.62857142857143" customWidth="1"/>
     <col min="2" max="2" width="12.247619047619" customWidth="1"/>
@@ -1643,50 +1488,43 @@
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A1" s="51"/>
-      <c r="B1" s="52" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:5">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
     </row>
     <row r="3" ht="18" customHeight="1" spans="1:5">
-      <c r="A3" s="53"/>
-      <c r="B3" s="55" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" ht="42" customHeight="1" spans="1:5">
-      <c r="A4" s="53"/>
-      <c r="B4" s="56" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="53" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" ht="21" customHeight="1" spans="1:5">
-      <c r="A5" s="53"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1705,7 +1543,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
@@ -1787,7 +1625,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" ht="19.5" customHeight="1" spans="1:2">
+    <row r="9" ht="45" customHeight="1" spans="1:2">
       <c r="A9" s="11"/>
       <c r="B9" s="15" t="s">
         <v>12</v>
@@ -1803,105 +1641,105 @@
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:6">
       <c r="A11" s="11"/>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" ht="19.5" customHeight="1" spans="1:6">
-      <c r="A12" s="50"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="28"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" ht="19.5" customHeight="1" spans="1:6">
-      <c r="A13" s="50"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="28"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" ht="19.5" hidden="1" customHeight="1" spans="1:6">
       <c r="A14" s="11"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35">
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34">
         <f t="shared" ref="F14:F18" si="0">PRODUCT(D14,E14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" ht="19.5" hidden="1" customHeight="1" spans="1:6">
       <c r="A15" s="11"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35">
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" ht="19.5" hidden="1" customHeight="1" spans="1:6">
       <c r="A16" s="11"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35">
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" ht="19.5" hidden="1" customHeight="1" spans="1:6">
       <c r="A17" s="11"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" ht="19.5" hidden="1" customHeight="1" spans="1:6">
       <c r="A18" s="11"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35">
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" ht="30" customHeight="1" spans="1:5">
-      <c r="A19" s="46"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="49"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
     </row>
     <row r="20" ht="19.5" customHeight="1" spans="1:6">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="34"/>
+      <c r="D20" s="43"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
     </row>
@@ -1929,10 +1767,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="6"/>
@@ -2023,7 +1861,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" ht="19.5" customHeight="1" spans="1:7">
+    <row r="9" ht="65" customHeight="1" spans="1:7">
       <c r="A9" s="11"/>
       <c r="B9" s="15" t="s">
         <v>18</v>
@@ -2173,164 +2011,93 @@
     <row r="27" ht="30" customHeight="1" spans="1:7">
       <c r="A27" s="11"/>
       <c r="B27" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="C27" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="32"/>
+      <c r="F27" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" ht="19.5" customHeight="1" spans="1:7">
       <c r="A28" s="11"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-    </row>
-    <row r="29" ht="19.5" hidden="1" customHeight="1" spans="1:7">
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+    </row>
+    <row r="29" ht="19.5" customHeight="1" spans="1:7">
       <c r="A29" s="11"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35">
-        <f t="shared" ref="F29:F33" si="0">PRODUCT(D29,E29)</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="35"/>
-    </row>
-    <row r="30" ht="19.5" hidden="1" customHeight="1" spans="1:7">
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+    </row>
+    <row r="30" ht="19.5" customHeight="1" spans="1:7">
       <c r="A30" s="11"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="35"/>
-    </row>
-    <row r="31" ht="19.5" hidden="1" customHeight="1" spans="1:7">
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+    </row>
+    <row r="31" ht="19.5" customHeight="1" spans="1:7">
       <c r="A31" s="11"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="35"/>
-    </row>
-    <row r="32" ht="19.5" hidden="1" customHeight="1" spans="1:7">
-      <c r="A32" s="11"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+    </row>
+    <row r="32" ht="18" customHeight="1" spans="1:7">
+      <c r="A32" s="12"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="36"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="35"/>
-    </row>
-    <row r="33" ht="19.5" hidden="1" customHeight="1" spans="1:7">
-      <c r="A33" s="11"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+    </row>
+    <row r="33" ht="18" customHeight="1" spans="1:7">
+      <c r="A33" s="12"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="36"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="35"/>
-    </row>
-    <row r="34" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A34" s="12"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="40">
-        <f>SUM(F28:F33)</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="41"/>
-    </row>
-    <row r="35" ht="18" customHeight="1" spans="1:7">
-      <c r="A35" s="12"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="F35" s="44">
-        <v>20</v>
-      </c>
-      <c r="G35" s="44"/>
-    </row>
-    <row r="36" ht="18" customHeight="1" spans="1:7">
-      <c r="A36" s="12"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" s="45">
-        <v>0.086</v>
-      </c>
-      <c r="G36" s="45"/>
-    </row>
-    <row r="37" ht="18" customHeight="1" spans="1:7">
-      <c r="A37" s="12"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F37" s="44">
-        <f>F34*F36</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="44"/>
-    </row>
-    <row r="38" ht="30" customHeight="1" spans="1:7">
-      <c r="A38" s="46"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="49">
-        <f>SUM(F34,F35,F37)</f>
-        <v>20</v>
-      </c>
-      <c r="G38" s="49"/>
-    </row>
-    <row r="39" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+    </row>
+    <row r="34" ht="30" customHeight="1" spans="1:7">
+      <c r="A34" s="39"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42"/>
+      <c r="G34" s="42"/>
+    </row>
+    <row r="35" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="40">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
@@ -2368,16 +2135,11 @@
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="E34:F34"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>